<commit_message>
excel reader will read missing cell as blank
</commit_message>
<xml_diff>
--- a/automationtest/src/test/resources/test.xlsx
+++ b/automationtest/src/test/resources/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\test_framework\automationtest\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA37D07-9B28-41A4-93E8-658085489E77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19F05C4-2ADC-40D1-8C8C-26FD6B8322C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,21 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>mngr248531</t>
-  </si>
-  <si>
-    <t>nYtUsEn</t>
-  </si>
-  <si>
     <t>linxiang08@gmail.com</t>
-  </si>
-  <si>
-    <t>123nn456</t>
   </si>
 </sst>
 </file>
@@ -369,16 +360,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -388,54 +376,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>111</v>
-      </c>
-      <c r="B2">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{527D6079-73C0-4C99-A709-EDF593DE1174}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1B61E0-0642-49E6-8996-27B72E684763}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A64AAA-1CBA-4CA7-A0CD-23FDEB6D0E01}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <v>123456</v>
@@ -443,7 +404,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{818FBF4F-F2F7-4B60-8C55-48B53437EE7B}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{51386623-7E7B-49EB-8057-D9EC8A9233A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>